<commit_message>
First pass at power calculations using simulation
</commit_message>
<xml_diff>
--- a/Stimuli/Phrase_Details.xlsx
+++ b/Stimuli/Phrase_Details.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
   <si>
     <t>Melody Code</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>Instrument</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>After</t>
   </si>
 </sst>
 </file>
@@ -651,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +676,7 @@
     <col min="6" max="6" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -689,8 +698,11 @@
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -712,8 +724,11 @@
       <c r="G2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -735,8 +750,11 @@
       <c r="G3">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -758,8 +776,11 @@
       <c r="G4">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -781,8 +802,11 @@
       <c r="G5">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -804,8 +828,11 @@
       <c r="G6">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -827,8 +854,11 @@
       <c r="G7">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -850,8 +880,11 @@
       <c r="G8">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -873,8 +906,11 @@
       <c r="G9">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -896,8 +932,11 @@
       <c r="G10">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -919,8 +958,11 @@
       <c r="G11">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -942,8 +984,11 @@
       <c r="G12">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -965,8 +1010,11 @@
       <c r="G13">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -988,8 +1036,11 @@
       <c r="G14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1011,8 +1062,11 @@
       <c r="G15">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1034,8 +1088,11 @@
       <c r="G16">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1056,6 +1113,9 @@
       </c>
       <c r="G17">
         <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on papaja manuscript
</commit_message>
<xml_diff>
--- a/Stimuli/Phrase_Details.xlsx
+++ b/Stimuli/Phrase_Details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Sauve\MUN Postdoc\Entropy-Learning-Atonal\Stimuli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Sauve\MUN Postdoc\Entropy-Learning-Atonal-Project\Stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Measures</t>
-  </si>
-  <si>
-    <t>Length (in notes)</t>
   </si>
   <si>
     <t>Dallapiccola_quartina_1</t>
@@ -325,6 +322,9 @@
   </si>
   <si>
     <t>After</t>
+  </si>
+  <si>
+    <t>Length</t>
   </si>
 </sst>
 </file>
@@ -663,7 +663,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +678,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -693,429 +693,429 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2">
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3">
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4">
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5">
         <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6">
         <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7">
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8">
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9">
         <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10">
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11">
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12">
         <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13">
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G14">
         <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G15">
         <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16">
         <v>13</v>
       </c>
       <c r="H16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G17">
         <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>